<commit_message>
making the gamma value calc code more robust
</commit_message>
<xml_diff>
--- a/CANELa_NP/Data/single_atom_energies.xlsx
+++ b/CANELa_NP/Data/single_atom_energies.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Denny/Desktop/Pitt/CANELA_Fall_2022/NP_Tools/CANELa/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Denny/Desktop/Pitt/CANELa_NP/CANELa_NP/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6347F831-BD6C-6745-B7C0-2A03DA0D84E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E2F4A1-E83D-A045-82C6-F51CAE11F2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{67DF3A7F-7A84-914D-8EC0-6C96B0D1632A}"/>
+    <workbookView xWindow="7200" yWindow="1680" windowWidth="19200" windowHeight="21100" xr2:uid="{67DF3A7F-7A84-914D-8EC0-6C96B0D1632A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>NP</t>
   </si>
@@ -50,6 +51,12 @@
   </si>
   <si>
     <t>Energy (Ha)</t>
+  </si>
+  <si>
+    <t>Ag</t>
+  </si>
+  <si>
+    <t>Cu</t>
   </si>
 </sst>
 </file>
@@ -407,7 +414,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,6 +455,24 @@
         <v>-33.138799651730999</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <f>-1004.93065412009/27.2114</f>
+        <v>-36.930501705905982</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>-1305.9228912226/27.2114</f>
+        <v>-47.991756808639018</v>
+      </c>
+    </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>